<commit_message>
Updated test cases adding negative test. Refactored code
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheila\source\repos\marsframework\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheila\source\repos\CompetitionTask\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4A7A03-C147-4518-991E-06C449893B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3EBA34-6E01-45AB-9DCB-92712B746FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1077,16 +1077,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CADAEA-313B-4C8F-8DA8-E7E3488AC4F3}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" customWidth="1"/>
+    <col min="1" max="1" width="34.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.6328125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="23.7265625" customWidth="1"/>
@@ -1212,11 +1212,9 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>128</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
         <v>46</v>
       </c>
@@ -1252,80 +1250,82 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N3" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="O3" t="str">
         <f>IF(N3=Data!$B$18,"Programming","")</f>
-        <v>Programming</v>
+        <v/>
       </c>
       <c r="P3" t="str">
         <f>IF(N3=Data!$B$19,"9","")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="Q3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11" t="s">
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="12" t="str">
-        <f>IFERROR(LEFT(C4,FIND(" ",C4)-1),C4)</f>
+      <c r="D5" s="12" t="str">
+        <f>IFERROR(LEFT(C5,FIND(" ",C5)-1),C5)</f>
         <v>Programming</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>47</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>48</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" t="s">
         <v>49</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H5" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I5" s="3">
         <v>45022</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J5" s="4">
         <v>45058</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L5" s="5">
         <v>0.75</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M5" s="5">
         <v>0.83333333333333337</v>
       </c>
-      <c r="N4" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" t="str">
-        <f>IF(N4=Data!$B$18,"Programming","")</f>
+      <c r="N5" t="s">
+        <v>111</v>
+      </c>
+      <c r="O5" t="str">
+        <f>IF(N5=Data!$B$18,"Programming","")</f>
+        <v>Programming</v>
+      </c>
+      <c r="P5" t="str">
+        <f>IF(N5=Data!$B$19,"9","")</f>
         <v/>
       </c>
-      <c r="P4" t="str">
-        <f>IF(N4=Data!$B$19,"9","")</f>
-        <v>9</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="Q5" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4" xr:uid="{0F853ED9-4439-469A-BD4D-CAC833F5874F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3 C5" xr:uid="{0F853ED9-4439-469A-BD4D-CAC833F5874F}">
       <formula1>Category</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{5BC4A312-96C5-43C9-8A36-22C362BC5909}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2 E3 E5" xr:uid="{5BC4A312-96C5-43C9-8A36-22C362BC5909}">
       <formula1>INDIRECT(SUBSTITUTE(D2," ",""))</formula1>
     </dataValidation>
   </dataValidations>
@@ -1338,31 +1338,31 @@
           <x14:formula1>
             <xm:f>Data!$B$18:$B$19</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N4</xm:sqref>
+          <xm:sqref>N2 N3 N5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CDED5CE9-BB5A-4BDE-B857-5395EE0E6AE7}">
           <x14:formula1>
             <xm:f>Data!$C$17:$C$18</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q4</xm:sqref>
+          <xm:sqref>Q2 Q3 Q5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FCE46D2E-E6E0-42CE-9078-7105969623F2}">
           <x14:formula1>
             <xm:f>Data!$D$17:$D$18</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H4</xm:sqref>
+          <xm:sqref>H2 H3 H5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B6C7974-F12B-4463-8DEA-A2A2FD13A67D}">
           <x14:formula1>
             <xm:f>Data!$E$17:$E$18</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G4</xm:sqref>
+          <xm:sqref>G2 G3 G5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AA3DF6C5-33E2-42C0-9CD6-0378A2FF10C1}">
           <x14:formula1>
             <xm:f>Data!$A$17:$A$23</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K4</xm:sqref>
+          <xm:sqref>K2 K3 K5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Test case added: Adding New Service with complete entries but with Invalid input
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheila\source\repos\CompetitionTask\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3EBA34-6E01-45AB-9DCB-92712B746FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EFA45B-B1F1-4568-9E5F-1D68DB4FC548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="132">
   <si>
     <t>Url</t>
   </si>
@@ -436,6 +436,15 @@
   </si>
   <si>
     <t>Edited Tutorial on the basics of Software Testing</t>
+  </si>
+  <si>
+    <t>The Basics of Software Testing</t>
+  </si>
+  <si>
+    <t>Software Testing: What You Need To Know</t>
+  </si>
+  <si>
+    <t>Software Testers Handbook</t>
   </si>
 </sst>
 </file>
@@ -1077,15 +1086,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CADAEA-313B-4C8F-8DA8-E7E3488AC4F3}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="34.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.6328125" hidden="1" customWidth="1"/>
@@ -1212,7 +1221,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
@@ -1264,12 +1273,68 @@
         <v>45</v>
       </c>
     </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="12" t="str">
+        <f>IFERROR(LEFT(C4,FIND(" ",C4)-1),C4)</f>
+        <v>Programming</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3">
+        <v>45022</v>
+      </c>
+      <c r="J4" s="4">
+        <v>45058</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="N4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" t="str">
+        <f>IF(N4=Data!$B$18,"Programming","")</f>
+        <v/>
+      </c>
+      <c r="P4" t="str">
+        <f>IF(N4=Data!$B$19,"9","")</f>
+        <v>9</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>46</v>
@@ -1306,26 +1371,147 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="N5" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="O5" t="str">
         <f>IF(N5=Data!$B$18,"Programming","")</f>
-        <v>Programming</v>
+        <v/>
       </c>
       <c r="P5" t="str">
         <f>IF(N5=Data!$B$19,"9","")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="Q5" t="s">
         <v>45</v>
       </c>
     </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="12" t="str">
+        <f>IFERROR(LEFT(C6,FIND(" ",C6)-1),C6)</f>
+        <v>Programming</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="3">
+        <v>45022</v>
+      </c>
+      <c r="J6" s="4">
+        <v>45058</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="N6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6" t="str">
+        <f>IF(N6=Data!$B$18,"Programming","")</f>
+        <v/>
+      </c>
+      <c r="P6" t="str">
+        <f>IF(N6=Data!$B$19,"9","")</f>
+        <v>9</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="12" t="str">
+        <f>IFERROR(LEFT(C8,FIND(" ",C8)-1),C8)</f>
+        <v>Programming</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="3">
+        <v>45022</v>
+      </c>
+      <c r="J8" s="4">
+        <v>45058</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="N8" t="s">
+        <v>111</v>
+      </c>
+      <c r="O8" t="str">
+        <f>IF(N8=Data!$B$18,"Programming","")</f>
+        <v>Programming</v>
+      </c>
+      <c r="P8" t="str">
+        <f>IF(N8=Data!$B$19,"9","")</f>
+        <v/>
+      </c>
+      <c r="Q8" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3 C5" xr:uid="{0F853ED9-4439-469A-BD4D-CAC833F5874F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3 C4:C8" xr:uid="{0F853ED9-4439-469A-BD4D-CAC833F5874F}">
       <formula1>Category</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2 E3 E5" xr:uid="{5BC4A312-96C5-43C9-8A36-22C362BC5909}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3 E4:E8" xr:uid="{5BC4A312-96C5-43C9-8A36-22C362BC5909}">
       <formula1>INDIRECT(SUBSTITUTE(D2," ",""))</formula1>
     </dataValidation>
   </dataValidations>
@@ -1338,31 +1524,31 @@
           <x14:formula1>
             <xm:f>Data!$B$18:$B$19</xm:f>
           </x14:formula1>
-          <xm:sqref>N2 N3 N5</xm:sqref>
+          <xm:sqref>N2:N3 N4:N8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CDED5CE9-BB5A-4BDE-B857-5395EE0E6AE7}">
           <x14:formula1>
             <xm:f>Data!$C$17:$C$18</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2 Q3 Q5</xm:sqref>
+          <xm:sqref>Q2:Q3 Q4:Q8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FCE46D2E-E6E0-42CE-9078-7105969623F2}">
           <x14:formula1>
             <xm:f>Data!$D$17:$D$18</xm:f>
           </x14:formula1>
-          <xm:sqref>H2 H3 H5</xm:sqref>
+          <xm:sqref>H2:H3 H4:H8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B6C7974-F12B-4463-8DEA-A2A2FD13A67D}">
           <x14:formula1>
             <xm:f>Data!$E$17:$E$18</xm:f>
           </x14:formula1>
-          <xm:sqref>G2 G3 G5</xm:sqref>
+          <xm:sqref>G2:G3 G4:G8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AA3DF6C5-33E2-42C0-9CD6-0378A2FF10C1}">
           <x14:formula1>
             <xm:f>Data!$A$17:$A$23</xm:f>
           </x14:formula1>
-          <xm:sqref>K2 K3 K5</xm:sqref>
+          <xm:sqref>K2:K3 K4:K8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>